<commit_message>
Made test 9 sort alg via decorator, some refactoring. Array data files. + xlsx - speed stats.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t xml:space="preserve">alg_inter_sort: </t>
   </si>
@@ -58,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -109,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -168,7 +168,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -287,10 +287,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -320,22 +320,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$M$2</c:f>
+              <c:f>Лист1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -365,12 +359,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.000093460083E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.0000209808349601E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.9931278228759696E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -441,10 +429,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -474,22 +462,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$3:$M$3</c:f>
+              <c:f>Лист1!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -519,12 +501,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.9997100830078099E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.9998245239257795E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.2001028060912999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -595,10 +571,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -628,22 +604,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$4:$M$4</c:f>
+              <c:f>Лист1!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1.9998550415039002E-3</c:v>
                 </c:pt>
@@ -673,12 +643,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.1000146865844699E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.1572093963622998E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.100959777832031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -749,10 +713,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -782,22 +746,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$5:$M$5</c:f>
+              <c:f>Лист1!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.2499561309814401E-3</c:v>
                 </c:pt>
@@ -827,12 +785,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>3.1443834304809501E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.7260026931762695E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.147152423858642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -903,10 +855,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -936,22 +888,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$6:$M$6</c:f>
+              <c:f>Лист1!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4.0071010589599601E-3</c:v>
                 </c:pt>
@@ -981,12 +927,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.6999454498291002E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.105831146240234</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.224956274032592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1057,10 +997,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1090,22 +1030,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$7:$M$7</c:f>
+              <c:f>Лист1!$B$7:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.9925785064697196E-3</c:v>
                 </c:pt>
@@ -1135,12 +1069,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>9.9552392959594699E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.21693325042724601</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.502033472061157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1216,10 +1144,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1249,22 +1177,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$8:$M$8</c:f>
+              <c:f>Лист1!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>4.2000055313110303E-2</c:v>
                 </c:pt>
@@ -1294,12 +1216,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.0411634445190403</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16.4758186340332</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>69.578309059142995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,10 +1291,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1408,22 +1324,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$9:$M$9</c:f>
+              <c:f>Лист1!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5.4000377655029297E-2</c:v>
                 </c:pt>
@@ -1453,12 +1363,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5.5305247306823704</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>23.153918743133499</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>90.735826015472398</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,10 +1438,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$M$1</c:f>
+              <c:f>Лист1!$B$1:$K$1</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1567,22 +1471,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$10:$M$10</c:f>
+              <c:f>Лист1!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.10057950019836399</c:v>
                 </c:pt>
@@ -1612,12 +1510,6 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10.743062257766701</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45.097231626510599</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>173.536309242248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1681,7 +1573,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="28814319"/>
@@ -1740,7 +1632,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="28812655"/>
@@ -1787,7 +1679,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="28814319"/>
@@ -1829,7 +1721,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1859,7 +1751,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1911,7 +1803,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1919,17 +1811,31 @@
     <c:view3D>
       <c:rotX val="15"/>
       <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
       <c:rAngAx val="0"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
-        <a:sp3d/>
+        <a:sp3d contourW="9525">
+          <a:contourClr>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:contourClr>
+        </a:sp3d>
       </c:spPr>
     </c:floor>
     <c:sideWall>
@@ -1956,7 +1862,7 @@
     </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:line3DChart>
+      <c:area3DChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -1964,7 +1870,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$2</c:f>
+              <c:f>Лист1!$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1985,116 +1891,85 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$P$1</c:f>
+              <c:f>Лист1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6000</c:v>
+                  <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>200000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$P$2</c:f>
+              <c:f>Лист1!$B$44:$K$44</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.7982959747314401E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.4964561462402302E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.5942773818969699E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8.1961870193481404E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2137889862060499E-3</c:v>
+                  <c:v>0.11088681221008299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0240077972412101E-3</c:v>
+                  <c:v>0.13686060905456501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.16802597045898399</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0013580322265599E-3</c:v>
+                  <c:v>0.19679832458495999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0103454589843698E-3</c:v>
+                  <c:v>0.228765964508056</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.000093460083E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.0000209808349601E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.9931278228759696E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6249418258666899E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.60031223297119E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.5001983642578097E-2</c:v>
+                  <c:v>0.26073288917541498</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2134-4368-A565-08DC4A8BCA81}"/>
+              <c16:uniqueId val="{00000000-57F9-43D6-B8B5-7477D0C5DF59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2103,7 +1978,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$3</c:f>
+              <c:f>Лист1!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2124,116 +1999,85 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$P$1</c:f>
+              <c:f>Лист1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6000</c:v>
+                  <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>200000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$3:$P$3</c:f>
+              <c:f>Лист1!$B$45:$K$45</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.3945302963256801E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.113883972167968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9992752075195291E-4</c:v>
+                  <c:v>0.17788171768188399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9998550415039002E-3</c:v>
+                  <c:v>0.24979567527770899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.00486183166503E-3</c:v>
+                  <c:v>0.32266974449157698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.97601318359375E-3</c:v>
+                  <c:v>0.40858197212219199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.000093460083E-3</c:v>
+                  <c:v>0.49556231498718201</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0146579742431597E-3</c:v>
+                  <c:v>0.57541108131408603</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.9909610748290998E-3</c:v>
+                  <c:v>0.65433049201965299</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9997100830078099E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.9998245239257795E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.2001028060912999E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.09989356994628E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.4999103546142495E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.134001970291137</c:v>
+                  <c:v>0.75223040580749501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2134-4368-A565-08DC4A8BCA81}"/>
+              <c16:uniqueId val="{00000001-57F9-43D6-B8B5-7477D0C5DF59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2242,7 +2086,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$4</c:f>
+              <c:f>Лист1!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2263,116 +2107,85 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$P$1</c:f>
+              <c:f>Лист1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6000</c:v>
+                  <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>200000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$4:$P$4</c:f>
+              <c:f>Лист1!$B$46:$K$46</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.9998550415039002E-3</c:v>
+                  <c:v>0.26572799682617099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0018558502197196E-3</c:v>
+                  <c:v>0.55742859840393</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2335262298583898E-3</c:v>
+                  <c:v>0.83720207214355402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0000419616699201E-3</c:v>
+                  <c:v>1.2064287662506099</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0001354217529297E-3</c:v>
+                  <c:v>1.5733907222747801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9999904632568307E-3</c:v>
+                  <c:v>1.92902660369873</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.20003223419189E-2</c:v>
+                  <c:v>2.31007599830627</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3993501663207999E-2</c:v>
+                  <c:v>2.6662721633911102</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.49996280670166E-2</c:v>
+                  <c:v>3.0458838939666699</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1000146865844699E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.1572093963622998E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.100959777832031</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.18636560440063399</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.347309350967407</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.62577295303344704</c:v>
+                  <c:v>4.2011799812316797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2134-4368-A565-08DC4A8BCA81}"/>
+              <c16:uniqueId val="{00000002-57F9-43D6-B8B5-7477D0C5DF59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2381,7 +2194,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$5</c:f>
+              <c:f>Лист1!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2402,116 +2215,85 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$P$1</c:f>
+              <c:f>Лист1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6000</c:v>
+                  <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>200000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$5:$P$5</c:f>
+              <c:f>Лист1!$B$47:$K$47</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.2499561309814401E-3</c:v>
+                  <c:v>0.45453453063964799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0015449523925703E-3</c:v>
+                  <c:v>0.88198518753051702</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0003738403320295E-3</c:v>
+                  <c:v>1.41910028457641</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.20000839233398E-2</c:v>
+                  <c:v>1.83012723922729</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.39997005462646E-2</c:v>
+                  <c:v>2.5613784790039</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6253709793090799E-2</c:v>
+                  <c:v>2.9811315536499001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.20000743865966E-2</c:v>
+                  <c:v>3.4524667263031001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3995161056518499E-2</c:v>
+                  <c:v>4.0408651828765798</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.6998519897460899E-2</c:v>
+                  <c:v>4.5053901672363201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1443834304809501E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6.7260026931762695E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.147152423858642</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.29592275619506803</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.452549457550048</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.82098484039306596</c:v>
+                  <c:v>4.9998841285705504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2134-4368-A565-08DC4A8BCA81}"/>
+              <c16:uniqueId val="{00000003-57F9-43D6-B8B5-7477D0C5DF59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2520,7 +2302,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$6</c:f>
+              <c:f>Лист1!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2541,116 +2323,85 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$P$1</c:f>
+              <c:f>Лист1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6000</c:v>
+                  <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>200000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$6:$P$6</c:f>
+              <c:f>Лист1!$B$48:$K$48</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.0071010589599601E-3</c:v>
+                  <c:v>0.67730879783630304</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0130100250244106E-3</c:v>
+                  <c:v>1.3736457824707</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.30002498626708E-2</c:v>
+                  <c:v>2.1658439636230402</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6999959945678701E-2</c:v>
+                  <c:v>2.94362449645996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.30002403259277E-2</c:v>
+                  <c:v>3.73817586898803</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.62835025787353E-2</c:v>
+                  <c:v>4.58036041259765</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.24597358703613E-2</c:v>
+                  <c:v>5.3735022544860804</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.6201477050781201E-2</c:v>
+                  <c:v>6.2176389694213796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.9017438888549798E-2</c:v>
+                  <c:v>7.0759952068328804</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.6999454498291002E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.105831146240234</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.224956274032592</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.479687690734863</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.72094464302062899</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.2640516757964999</c:v>
+                  <c:v>7.9202404022216797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-2134-4368-A565-08DC4A8BCA81}"/>
+              <c16:uniqueId val="{00000004-57F9-43D6-B8B5-7477D0C5DF59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2659,7 +2410,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$A$7</c:f>
+              <c:f>Лист1!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2680,116 +2431,85 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$1:$P$1</c:f>
+              <c:f>Лист1!$B$43:$K$43</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2000</c:v>
+                  <c:v>200000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3000</c:v>
+                  <c:v>300000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4000</c:v>
+                  <c:v>400000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5000</c:v>
+                  <c:v>500000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6000</c:v>
+                  <c:v>600000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7000</c:v>
+                  <c:v>700000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8000</c:v>
+                  <c:v>800000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9000</c:v>
+                  <c:v>900000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>200000</c:v>
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$7:$P$7</c:f>
+              <c:f>Лист1!$B$49:$K$49</c:f>
               <c:numCache>
                 <c:formatCode>#\ ##0.0000000000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.9925785064697196E-3</c:v>
+                  <c:v>1.4295358657836901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6993284225463801E-2</c:v>
+                  <c:v>2.90835213661193</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.59995460510253E-2</c:v>
+                  <c:v>4.5205345153808496</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.50000858306884E-2</c:v>
+                  <c:v>6.1666898727416903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4963598251342697E-2</c:v>
+                  <c:v>7.81400442123413</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5000543594360303E-2</c:v>
+                  <c:v>9.5712528228759695</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.2538137435913003E-2</c:v>
+                  <c:v>11.261477470397899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9238414764404297E-2</c:v>
+                  <c:v>13.028669834136901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.2027673721313393E-2</c:v>
+                  <c:v>15.053035020828201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.9552392959594699E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.21693325042724601</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.502033472061157</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0143079757690401</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.5473620891571001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2.6977026462554901</c:v>
+                  <c:v>16.716282129287698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-2134-4368-A565-08DC4A8BCA81}"/>
+              <c16:uniqueId val="{00000005-57F9-43D6-B8B5-7477D0C5DF59}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2801,12 +2521,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="617716799"/>
-        <c:axId val="617720959"/>
-        <c:axId val="34966079"/>
-      </c:line3DChart>
+        <c:axId val="2095937488"/>
+        <c:axId val="2095942064"/>
+        <c:axId val="1790611360"/>
+      </c:area3DChart>
       <c:catAx>
-        <c:axId val="617716799"/>
+        <c:axId val="2095937488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,10 +2566,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617720959"/>
+        <c:crossAx val="2095942064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2857,7 +2577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="617720959"/>
+        <c:axId val="2095942064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2905,15 +2625,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617716799"/>
+        <c:crossAx val="2095937488"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="34966079"/>
+        <c:axId val="1790611360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2952,10 +2672,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617720959"/>
+        <c:crossAx val="2095942064"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -2994,12 +2714,12 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -3024,7 +2744,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3641,7 +3361,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="307">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="276">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3911,9 +3631,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:floor>
@@ -4161,15 +3886,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>21430</xdr:colOff>
+      <xdr:colOff>21429</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>45242</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>490536</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
+      <xdr:colOff>866774</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4191,19 +3916,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>26192</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>92867</xdr:rowOff>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4484,24 +4209,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:K49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1000</v>
@@ -4533,23 +4257,8 @@
       <c r="K1" s="2">
         <v>10000</v>
       </c>
-      <c r="L1" s="2">
-        <v>20000</v>
-      </c>
-      <c r="M1" s="2">
-        <v>40000</v>
-      </c>
-      <c r="N1" s="2">
-        <v>80000</v>
-      </c>
-      <c r="O1" s="2">
-        <v>120000</v>
-      </c>
-      <c r="P1" s="2">
-        <v>200000</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4583,23 +4292,8 @@
       <c r="K2" s="3">
         <v>2.000093460083E-3</v>
       </c>
-      <c r="L2" s="3">
-        <v>3.0000209808349601E-3</v>
-      </c>
-      <c r="M2" s="3">
-        <v>5.9931278228759696E-3</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1.6249418258666899E-2</v>
-      </c>
-      <c r="O2" s="3">
-        <v>2.60031223297119E-2</v>
-      </c>
-      <c r="P2" s="3">
-        <v>4.5001983642578097E-2</v>
-      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4633,23 +4327,8 @@
       <c r="K3" s="3">
         <v>3.9997100830078099E-3</v>
       </c>
-      <c r="L3" s="3">
-        <v>8.9998245239257795E-3</v>
-      </c>
-      <c r="M3" s="3">
-        <v>2.2001028060912999E-2</v>
-      </c>
-      <c r="N3" s="3">
-        <v>4.09989356994628E-2</v>
-      </c>
-      <c r="O3" s="3">
-        <v>6.4999103546142495E-2</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0.134001970291137</v>
-      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4683,23 +4362,8 @@
       <c r="K4" s="3">
         <v>2.1000146865844699E-2</v>
       </c>
-      <c r="L4" s="3">
-        <v>4.1572093963622998E-2</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.100959777832031</v>
-      </c>
-      <c r="N4" s="3">
-        <v>0.18636560440063399</v>
-      </c>
-      <c r="O4" s="3">
-        <v>0.347309350967407</v>
-      </c>
-      <c r="P4" s="3">
-        <v>0.62577295303344704</v>
-      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4733,23 +4397,8 @@
       <c r="K5" s="3">
         <v>3.1443834304809501E-2</v>
       </c>
-      <c r="L5" s="3">
-        <v>6.7260026931762695E-2</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0.147152423858642</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0.29592275619506803</v>
-      </c>
-      <c r="O5" s="3">
-        <v>0.452549457550048</v>
-      </c>
-      <c r="P5" s="3">
-        <v>0.82098484039306596</v>
-      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4783,23 +4432,8 @@
       <c r="K6" s="3">
         <v>4.6999454498291002E-2</v>
       </c>
-      <c r="L6" s="3">
-        <v>0.105831146240234</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.224956274032592</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.479687690734863</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.72094464302062899</v>
-      </c>
-      <c r="P6" s="3">
-        <v>1.2640516757964999</v>
-      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -4833,23 +4467,8 @@
       <c r="K7" s="3">
         <v>9.9552392959594699E-2</v>
       </c>
-      <c r="L7" s="3">
-        <v>0.21693325042724601</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0.502033472061157</v>
-      </c>
-      <c r="N7" s="3">
-        <v>1.0143079757690401</v>
-      </c>
-      <c r="O7" s="3">
-        <v>1.5473620891571001</v>
-      </c>
-      <c r="P7" s="3">
-        <v>2.6977026462554901</v>
-      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -4883,14 +4502,8 @@
       <c r="K8" s="3">
         <v>4.0411634445190403</v>
       </c>
-      <c r="L8" s="3">
-        <v>16.4758186340332</v>
-      </c>
-      <c r="M8" s="3">
-        <v>69.578309059142995</v>
-      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4924,14 +4537,8 @@
       <c r="K9" s="3">
         <v>5.5305247306823704</v>
       </c>
-      <c r="L9" s="3">
-        <v>23.153918743133499</v>
-      </c>
-      <c r="M9" s="3">
-        <v>90.735826015472398</v>
-      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4965,16 +4572,262 @@
       <c r="K10" s="3">
         <v>10.743062257766701</v>
       </c>
-      <c r="L10" s="3">
-        <v>45.097231626510599</v>
-      </c>
-      <c r="M10" s="3">
-        <v>173.536309242248</v>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2">
+        <v>100000</v>
+      </c>
+      <c r="C43" s="2">
+        <f>B43+100000</f>
+        <v>200000</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" ref="D43:K43" si="0">C43+100000</f>
+        <v>300000</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="0"/>
+        <v>400000</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" si="0"/>
+        <v>500000</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="0"/>
+        <v>600000</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="0"/>
+        <v>700000</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="0"/>
+        <v>800000</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="0"/>
+        <v>900000</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1.7982959747314401E-2</v>
+      </c>
+      <c r="C44" s="3">
+        <v>3.4964561462402302E-2</v>
+      </c>
+      <c r="D44" s="3">
+        <v>5.5942773818969699E-2</v>
+      </c>
+      <c r="E44" s="3">
+        <v>8.1961870193481404E-2</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.11088681221008299</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0.13686060905456501</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0.16802597045898399</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0.19679832458495999</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0.228765964508056</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0.26073288917541498</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="3">
+        <v>5.3945302963256801E-2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.113883972167968</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.17788171768188399</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.24979567527770899</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.32266974449157698</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.40858197212219199</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0.49556231498718201</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0.57541108131408603</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0.65433049201965299</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0.75223040580749501</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0.26572799682617099</v>
+      </c>
+      <c r="C46" s="3">
+        <v>0.55742859840393</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0.83720207214355402</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1.2064287662506099</v>
+      </c>
+      <c r="F46" s="3">
+        <v>1.5733907222747801</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1.92902660369873</v>
+      </c>
+      <c r="H46" s="3">
+        <v>2.31007599830627</v>
+      </c>
+      <c r="I46" s="3">
+        <v>2.6662721633911102</v>
+      </c>
+      <c r="J46" s="3">
+        <v>3.0458838939666699</v>
+      </c>
+      <c r="K46" s="3">
+        <v>4.2011799812316797</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0.45453453063964799</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.88198518753051702</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.41910028457641</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1.83012723922729</v>
+      </c>
+      <c r="F47" s="3">
+        <v>2.5613784790039</v>
+      </c>
+      <c r="G47" s="3">
+        <v>2.9811315536499001</v>
+      </c>
+      <c r="H47" s="3">
+        <v>3.4524667263031001</v>
+      </c>
+      <c r="I47" s="3">
+        <v>4.0408651828765798</v>
+      </c>
+      <c r="J47" s="3">
+        <v>4.5053901672363201</v>
+      </c>
+      <c r="K47" s="3">
+        <v>4.9998841285705504</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0.67730879783630304</v>
+      </c>
+      <c r="C48" s="3">
+        <v>1.3736457824707</v>
+      </c>
+      <c r="D48" s="3">
+        <v>2.1658439636230402</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2.94362449645996</v>
+      </c>
+      <c r="F48" s="3">
+        <v>3.73817586898803</v>
+      </c>
+      <c r="G48" s="3">
+        <v>4.58036041259765</v>
+      </c>
+      <c r="H48" s="3">
+        <v>5.3735022544860804</v>
+      </c>
+      <c r="I48" s="3">
+        <v>6.2176389694213796</v>
+      </c>
+      <c r="J48" s="3">
+        <v>7.0759952068328804</v>
+      </c>
+      <c r="K48" s="3">
+        <v>7.9202404022216797</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1.4295358657836901</v>
+      </c>
+      <c r="C49" s="3">
+        <v>2.90835213661193</v>
+      </c>
+      <c r="D49" s="3">
+        <v>4.5205345153808496</v>
+      </c>
+      <c r="E49" s="3">
+        <v>6.1666898727416903</v>
+      </c>
+      <c r="F49" s="3">
+        <v>7.81400442123413</v>
+      </c>
+      <c r="G49" s="3">
+        <v>9.5712528228759695</v>
+      </c>
+      <c r="H49" s="3">
+        <v>11.261477470397899</v>
+      </c>
+      <c r="I49" s="3">
+        <v>13.028669834136901</v>
+      </c>
+      <c r="J49" s="3">
+        <v>15.053035020828201</v>
+      </c>
+      <c r="K49" s="3">
+        <v>16.716282129287698</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>